<commit_message>
Terminplan angepasst, Expose berichtigt (Version 2.1)
</commit_message>
<xml_diff>
--- a/Terminplan_Bachelorarbeit.xlsx
+++ b/Terminplan_Bachelorarbeit.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian Helberg\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\bachelor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6AA555-2C83-4A0C-94F0-EB41B78D5820}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C5207F-01E7-4AD6-A69A-F9DADF6DA5D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{A4AB81FD-19AB-4952-B83D-6CD5816E8924}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Montag</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Kolloquium</t>
+  </si>
+  <si>
+    <t>Geblockt</t>
   </si>
 </sst>
 </file>
@@ -136,7 +139,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,6 +206,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -296,10 +305,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -312,35 +320,30 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="14" fontId="3" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884FB549-0994-4EA9-A0E2-34E2A8E94A31}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A17" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,301 +726,301 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21">
+      <c r="A2" s="17">
         <v>44088</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="12">
         <v>44089</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="11">
         <v>44090</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="11">
         <v>44091</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="11">
         <v>44092</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="11">
         <v>44093</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="11">
         <v>44094</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16">
+      <c r="A3" s="14">
         <v>44095</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>44096</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <v>44097</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="11">
         <v>44098</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <v>44099</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="11">
         <v>44100</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11">
         <v>44101</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22">
+      <c r="A4" s="18">
         <v>44102</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="12">
         <v>44103</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="11">
         <v>44104</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="11">
         <v>44105</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="11">
         <v>44106</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="11">
         <v>44107</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="11">
         <v>44108</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18">
+      <c r="A5" s="14">
         <v>44109</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="11">
         <v>44110</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="11">
         <v>44111</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="11">
         <v>44112</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="11">
         <v>44113</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="11">
         <v>44114</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="11">
         <v>44115</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23">
+      <c r="A6" s="18">
         <v>44116</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="12">
         <v>44117</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="11">
         <v>44118</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="11">
         <v>44119</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="11">
         <v>44120</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="16">
         <v>44121</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="16">
         <v>44122</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="27">
+      <c r="A7" s="15">
         <v>44123</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="16">
         <v>44124</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="16">
         <v>44125</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="31">
         <v>44126</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="31">
         <v>44127</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="16">
         <v>44128</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="16">
         <v>44129</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29">
+      <c r="A8" s="33">
         <v>44130</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="19">
         <v>44131</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="20">
         <v>44132</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="20">
         <v>44133</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="20">
         <v>44134</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="20">
         <v>44135</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="20">
         <v>44136</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30">
+      <c r="A9" s="21">
         <v>44137</v>
       </c>
-      <c r="B9" s="31">
+      <c r="B9" s="22">
         <v>44138</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="22">
         <v>44139</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="22">
         <v>44140</v>
       </c>
-      <c r="E9" s="31">
+      <c r="E9" s="22">
         <v>44141</v>
       </c>
-      <c r="F9" s="31">
+      <c r="F9" s="22">
         <v>44142</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G9" s="22">
         <v>44143</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="33">
+      <c r="A10" s="24">
         <v>44144</v>
       </c>
-      <c r="B10" s="34">
+      <c r="B10" s="23">
         <v>44145</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="22">
         <v>44146</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="22">
         <v>44147</v>
       </c>
-      <c r="E10" s="35">
+      <c r="E10" s="22">
         <v>44148</v>
       </c>
-      <c r="F10" s="35">
+      <c r="F10" s="22">
         <v>44149</v>
       </c>
-      <c r="G10" s="35">
+      <c r="G10" s="22">
         <v>44150</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="36">
+      <c r="A11" s="21">
         <v>44151</v>
       </c>
-      <c r="B11" s="35">
+      <c r="B11" s="22">
         <v>44152</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="22">
         <v>44153</v>
       </c>
-      <c r="D11" s="35">
+      <c r="D11" s="22">
         <v>44154</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="22">
         <v>44155</v>
       </c>
-      <c r="F11" s="35">
+      <c r="F11" s="22">
         <v>44156</v>
       </c>
-      <c r="G11" s="35">
+      <c r="G11" s="22">
         <v>44157</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37">
+      <c r="A12" s="24">
         <v>44158</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="23">
         <v>44159</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="22">
         <v>44160</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="22">
         <v>44161</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="22">
         <v>44162</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="22">
         <v>44163</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="22">
         <v>44164</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17">
+      <c r="A13" s="21">
         <v>44165</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="22">
         <v>44166</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="22">
         <v>44167</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="22">
         <v>44168</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="22">
         <v>44169</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="22">
         <v>44170</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="22">
         <v>44171</v>
       </c>
     </row>
@@ -1025,45 +1028,45 @@
       <c r="A14" s="24">
         <v>44172</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="23">
         <v>44173</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="22">
         <v>44174</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="22">
         <v>44175</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="22">
         <v>44176</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="22">
         <v>44177</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="22">
         <v>44178</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17">
+      <c r="A15" s="21">
         <v>44179</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="22">
         <v>44180</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="22">
         <v>44181</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="22">
         <v>44182</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="22">
         <v>44183</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="22">
         <v>44184</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="22">
         <v>44185</v>
       </c>
     </row>
@@ -1071,229 +1074,229 @@
       <c r="A16" s="24">
         <v>44186</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="23">
         <v>44187</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="22">
         <v>44188</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="22">
         <v>44189</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="22">
         <v>44190</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="22">
         <v>44191</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="22">
         <v>44192</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17">
+      <c r="A17" s="21">
         <v>44193</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="22">
         <v>44194</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="22">
         <v>44195</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="31">
         <v>44196</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="31">
         <v>44197</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="36">
         <v>44198</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="36">
         <v>44199</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="24">
+      <c r="A18" s="34">
         <v>44200</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="35">
         <v>44201</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="36">
         <v>44202</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="36">
         <v>44203</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="36">
         <v>44204</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="36">
         <v>44205</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="36">
         <v>44206</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17">
+      <c r="A19" s="37">
         <v>44207</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="36">
         <v>44208</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="36">
         <v>44209</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="36">
         <v>44210</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="36">
         <v>44211</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="36">
         <v>44212</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="36">
         <v>44213</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="24">
+      <c r="A20" s="34">
         <v>44214</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="35">
         <v>44215</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="36">
         <v>44216</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="36">
         <v>44217</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="36">
         <v>44218</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="36">
         <v>44219</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="36">
         <v>44220</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="17">
+      <c r="A21" s="37">
         <v>44221</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="36">
         <v>44222</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="36">
         <v>44223</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="36">
         <v>44224</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="36">
         <v>44225</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="36">
         <v>44226</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="36">
         <v>44227</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="24">
+      <c r="A22" s="34">
         <v>44228</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="35">
         <v>44229</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="36">
         <v>44230</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="36">
         <v>44231</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="36">
         <v>44232</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="36">
         <v>44233</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="36">
         <v>44234</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="17">
+      <c r="A23" s="37">
         <v>44235</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="36">
         <v>44236</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="36">
         <v>44237</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="36">
         <v>44238</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="36">
         <v>44239</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="36">
         <v>44240</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="36">
         <v>44241</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="39">
+      <c r="A24" s="25">
         <v>44242</v>
       </c>
-      <c r="B24" s="40">
+      <c r="B24" s="26">
         <v>44243</v>
       </c>
-      <c r="C24" s="41">
+      <c r="C24" s="27">
         <v>44244</v>
       </c>
-      <c r="D24" s="41">
+      <c r="D24" s="27">
         <v>44245</v>
       </c>
-      <c r="E24" s="41">
+      <c r="E24" s="27">
         <v>44246</v>
       </c>
-      <c r="F24" s="41">
+      <c r="F24" s="27">
         <v>44247</v>
       </c>
-      <c r="G24" s="41">
+      <c r="G24" s="27">
         <v>44248</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="42">
+      <c r="A25" s="28">
         <v>44249</v>
       </c>
-      <c r="B25" s="41">
+      <c r="B25" s="27">
         <v>44250</v>
       </c>
-      <c r="C25" s="41">
+      <c r="C25" s="27">
         <v>44251</v>
       </c>
-      <c r="D25" s="41">
+      <c r="D25" s="27">
         <v>44252</v>
       </c>
-      <c r="E25" s="41">
+      <c r="E25" s="27">
         <v>44253</v>
       </c>
-      <c r="F25" s="41">
+      <c r="F25" s="27">
         <v>44254</v>
       </c>
-      <c r="G25" s="41">
+      <c r="G25" s="27">
         <v>44255</v>
       </c>
     </row>
@@ -1329,7 +1332,7 @@
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="F29" s="43" t="s">
+      <c r="F29" s="29" t="s">
         <v>21</v>
       </c>
       <c r="G29" s="1"/>
@@ -1340,7 +1343,9 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+      <c r="F30" s="32" t="s">
+        <v>22</v>
+      </c>
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1555,29 +1560,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="30" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="30"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
@@ -1585,21 +1590,21 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="30" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="30"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B7" t="s">
@@ -1607,7 +1612,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B8" t="s">

</xml_diff>